<commit_message>
Added 2019 version with GR sector definitions
</commit_message>
<xml_diff>
--- a/projects/IOdata/data/GR2018_mappings.xlsx
+++ b/projects/IOdata/data/GR2018_mappings.xlsx
@@ -1148,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F147"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2614,9 +2614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4745,7 +4743,7 @@
   <dimension ref="A9:XFD43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>